<commit_message>
finish part A project 1
</commit_message>
<xml_diff>
--- a/data_624/ATM_Forecasts.xlsx
+++ b/data_624/ATM_Forecasts.xlsx
@@ -368,7 +368,7 @@
   <sheetViews>
     <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="1"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
@@ -730,7 +730,7 @@
         <v>4</v>
       </c>
       <c r="C33" t="n">
-        <v>66.4367753943482</v>
+        <v>66.4367753903359</v>
       </c>
     </row>
     <row r="34">
@@ -741,7 +741,7 @@
         <v>4</v>
       </c>
       <c r="C34" t="n">
-        <v>72.7179299235627</v>
+        <v>72.7179299344199</v>
       </c>
     </row>
     <row r="35">
@@ -752,7 +752,7 @@
         <v>4</v>
       </c>
       <c r="C35" t="n">
-        <v>13.6747888915319</v>
+        <v>13.6747888873261</v>
       </c>
     </row>
     <row r="36">
@@ -763,7 +763,7 @@
         <v>4</v>
       </c>
       <c r="C36" t="n">
-        <v>5.29799525314691</v>
+        <v>5.29799523543478</v>
       </c>
     </row>
     <row r="37">
@@ -774,7 +774,7 @@
         <v>4</v>
       </c>
       <c r="C37" t="n">
-        <v>97.6340457070469</v>
+        <v>97.6340457173049</v>
       </c>
     </row>
     <row r="38">
@@ -785,7 +785,7 @@
         <v>4</v>
       </c>
       <c r="C38" t="n">
-        <v>88.290341749614</v>
+        <v>88.2903417683511</v>
       </c>
     </row>
     <row r="39">
@@ -796,7 +796,7 @@
         <v>4</v>
       </c>
       <c r="C39" t="n">
-        <v>64.9889243966907</v>
+        <v>64.9889243970379</v>
       </c>
     </row>
     <row r="40">
@@ -807,7 +807,7 @@
         <v>4</v>
       </c>
       <c r="C40" t="n">
-        <v>66.4444427086188</v>
+        <v>66.4444427041864</v>
       </c>
     </row>
     <row r="41">
@@ -818,7 +818,7 @@
         <v>4</v>
       </c>
       <c r="C41" t="n">
-        <v>72.7270227656732</v>
+        <v>72.7270227773593</v>
       </c>
     </row>
     <row r="42">
@@ -829,7 +829,7 @@
         <v>4</v>
       </c>
       <c r="C42" t="n">
-        <v>13.6638606962407</v>
+        <v>13.6638606920493</v>
       </c>
     </row>
     <row r="43">
@@ -840,7 +840,7 @@
         <v>4</v>
       </c>
       <c r="C43" t="n">
-        <v>5.29441437218227</v>
+        <v>5.29441435371575</v>
       </c>
     </row>
     <row r="44">
@@ -851,7 +851,7 @@
         <v>4</v>
       </c>
       <c r="C44" t="n">
-        <v>97.6455699760028</v>
+        <v>97.6455699865798</v>
       </c>
     </row>
     <row r="45">
@@ -862,7 +862,7 @@
         <v>4</v>
       </c>
       <c r="C45" t="n">
-        <v>88.2886327470472</v>
+        <v>88.2886327663247</v>
       </c>
     </row>
     <row r="46">
@@ -873,7 +873,7 @@
         <v>4</v>
       </c>
       <c r="C46" t="n">
-        <v>64.9791410729403</v>
+        <v>64.9791410727616</v>
       </c>
     </row>
     <row r="47">
@@ -884,7 +884,7 @@
         <v>4</v>
       </c>
       <c r="C47" t="n">
-        <v>66.4502292791583</v>
+        <v>66.4502292744699</v>
       </c>
     </row>
     <row r="48">
@@ -895,7 +895,7 @@
         <v>4</v>
       </c>
       <c r="C48" t="n">
-        <v>72.7334551634686</v>
+        <v>72.7334551757421</v>
       </c>
     </row>
     <row r="49">
@@ -906,7 +906,7 @@
         <v>4</v>
       </c>
       <c r="C49" t="n">
-        <v>13.6557988842007</v>
+        <v>13.6557988799814</v>
       </c>
     </row>
     <row r="50">
@@ -917,7 +917,7 @@
         <v>4</v>
       </c>
       <c r="C50" t="n">
-        <v>5.2920242229896</v>
+        <v>5.29202420400523</v>
       </c>
     </row>
     <row r="51">
@@ -928,7 +928,7 @@
         <v>4</v>
       </c>
       <c r="C51" t="n">
-        <v>97.6539628742645</v>
+        <v>97.6539628850952</v>
       </c>
     </row>
     <row r="52">
@@ -939,7 +939,7 @@
         <v>4</v>
       </c>
       <c r="C52" t="n">
-        <v>88.2871893224936</v>
+        <v>88.2871893421265</v>
       </c>
     </row>
     <row r="53">
@@ -950,7 +950,7 @@
         <v>4</v>
       </c>
       <c r="C53" t="n">
-        <v>64.9721019460529</v>
+        <v>64.9721019454884</v>
       </c>
     </row>
     <row r="54">
@@ -961,7 +961,7 @@
         <v>4</v>
       </c>
       <c r="C54" t="n">
-        <v>66.4545879232397</v>
+        <v>66.4545879184008</v>
       </c>
     </row>
     <row r="55">
@@ -972,7 +972,7 @@
         <v>4</v>
       </c>
       <c r="C55" t="n">
-        <v>72.7379989703601</v>
+        <v>72.7379989830483</v>
       </c>
     </row>
     <row r="56">
@@ -983,7 +983,7 @@
         <v>4</v>
       </c>
       <c r="C56" t="n">
-        <v>13.649856605863</v>
+        <v>13.6498566015963</v>
       </c>
     </row>
     <row r="57">
@@ -994,7 +994,7 @@
         <v>4</v>
       </c>
       <c r="C57" t="n">
-        <v>5.2904427367059</v>
+        <v>5.29044271736816</v>
       </c>
     </row>
     <row r="58">
@@ -1005,7 +1005,7 @@
         <v>4</v>
       </c>
       <c r="C58" t="n">
-        <v>97.6600713195443</v>
+        <v>97.660071330574</v>
       </c>
     </row>
     <row r="59">
@@ -1016,7 +1016,7 @@
         <v>4</v>
       </c>
       <c r="C59" t="n">
-        <v>88.2859944457599</v>
+        <v>88.2859944656238</v>
       </c>
     </row>
     <row r="60">
@@ -1027,7 +1027,7 @@
         <v>4</v>
       </c>
       <c r="C60" t="n">
-        <v>64.9670411419784</v>
+        <v>64.9670411411321</v>
       </c>
     </row>
     <row r="61">
@@ -1038,7 +1038,7 @@
         <v>4</v>
       </c>
       <c r="C61" t="n">
-        <v>66.4578650363851</v>
+        <v>66.4578650314624</v>
       </c>
     </row>
     <row r="62">
@@ -1049,7 +1049,7 @@
         <v>4</v>
       </c>
       <c r="C62" t="n">
-        <v>72.7412037867213</v>
+        <v>72.7412037997009</v>
       </c>
     </row>
     <row r="63">
@@ -1060,7 +1060,7 @@
         <v>4</v>
       </c>
       <c r="C63" t="n">
-        <v>13.6454801843633</v>
+        <v>13.6454801800431</v>
       </c>
     </row>
     <row r="64">
@@ -1412,7 +1412,7 @@
         <v>6</v>
       </c>
       <c r="C95" t="n">
-        <v>361.262473359038</v>
+        <v>361.262473358633</v>
       </c>
     </row>
     <row r="96">
@@ -1423,7 +1423,7 @@
         <v>6</v>
       </c>
       <c r="C96" t="n">
-        <v>432.112991277724</v>
+        <v>432.112991277834</v>
       </c>
     </row>
     <row r="97">
@@ -1434,7 +1434,7 @@
         <v>6</v>
       </c>
       <c r="C97" t="n">
-        <v>450.32534646248</v>
+        <v>450.325346462679</v>
       </c>
     </row>
     <row r="98">
@@ -1445,7 +1445,7 @@
         <v>6</v>
       </c>
       <c r="C98" t="n">
-        <v>365.336628486316</v>
+        <v>365.336628486418</v>
       </c>
     </row>
     <row r="99">
@@ -1456,7 +1456,7 @@
         <v>6</v>
       </c>
       <c r="C99" t="n">
-        <v>426.577430254649</v>
+        <v>426.577430254802</v>
       </c>
     </row>
     <row r="100">
@@ -1467,7 +1467,7 @@
         <v>6</v>
       </c>
       <c r="C100" t="n">
-        <v>370.929346087746</v>
+        <v>370.929346087853</v>
       </c>
     </row>
     <row r="101">
@@ -1478,7 +1478,7 @@
         <v>6</v>
       </c>
       <c r="C101" t="n">
-        <v>451.125847023607</v>
+        <v>451.12584702378</v>
       </c>
     </row>
     <row r="102">
@@ -1489,7 +1489,7 @@
         <v>6</v>
       </c>
       <c r="C102" t="n">
-        <v>428.968708164577</v>
+        <v>428.968708164657</v>
       </c>
     </row>
     <row r="103">
@@ -1500,7 +1500,7 @@
         <v>6</v>
       </c>
       <c r="C103" t="n">
-        <v>441.939991101404</v>
+        <v>441.93999110159</v>
       </c>
     </row>
     <row r="104">
@@ -1511,7 +1511,7 @@
         <v>6</v>
       </c>
       <c r="C104" t="n">
-        <v>445.274301406921</v>
+        <v>445.274301407126</v>
       </c>
     </row>
     <row r="105">
@@ -1522,7 +1522,7 @@
         <v>6</v>
       </c>
       <c r="C105" t="n">
-        <v>429.714602766859</v>
+        <v>429.714602767033</v>
       </c>
     </row>
     <row r="106">
@@ -1533,7 +1533,7 @@
         <v>6</v>
       </c>
       <c r="C106" t="n">
-        <v>440.92654292412</v>
+        <v>440.926542924312</v>
       </c>
     </row>
     <row r="107">
@@ -1544,7 +1544,7 @@
         <v>6</v>
       </c>
       <c r="C107" t="n">
-        <v>430.738515146401</v>
+        <v>430.738515146577</v>
       </c>
     </row>
     <row r="108">
@@ -1555,7 +1555,7 @@
         <v>6</v>
       </c>
       <c r="C108" t="n">
-        <v>445.420856712013</v>
+        <v>445.420856712213</v>
       </c>
     </row>
     <row r="109">
@@ -1566,7 +1566,7 @@
         <v>6</v>
       </c>
       <c r="C109" t="n">
-        <v>441.364337075263</v>
+        <v>441.364337075442</v>
       </c>
     </row>
     <row r="110">
@@ -1577,7 +1577,7 @@
         <v>6</v>
       </c>
       <c r="C110" t="n">
-        <v>443.739114084237</v>
+        <v>443.739114084438</v>
       </c>
     </row>
     <row r="111">
@@ -1588,7 +1588,7 @@
         <v>6</v>
       </c>
       <c r="C111" t="n">
-        <v>444.349558208607</v>
+        <v>444.349558208812</v>
       </c>
     </row>
     <row r="112">
@@ -1599,7 +1599,7 @@
         <v>6</v>
       </c>
       <c r="C112" t="n">
-        <v>441.500895144441</v>
+        <v>441.500895144638</v>
       </c>
     </row>
     <row r="113">
@@ -1610,7 +1610,7 @@
         <v>6</v>
       </c>
       <c r="C113" t="n">
-        <v>443.553572419398</v>
+        <v>443.5535724196</v>
       </c>
     </row>
     <row r="114">
@@ -1621,7 +1621,7 @@
         <v>6</v>
       </c>
       <c r="C114" t="n">
-        <v>441.688352591016</v>
+        <v>441.688352591213</v>
       </c>
     </row>
     <row r="115">
@@ -1632,7 +1632,7 @@
         <v>6</v>
       </c>
       <c r="C115" t="n">
-        <v>444.376389492048</v>
+        <v>444.376389492252</v>
       </c>
     </row>
     <row r="116">
@@ -1643,7 +1643,7 @@
         <v>6</v>
       </c>
       <c r="C116" t="n">
-        <v>443.633723587934</v>
+        <v>443.633723588133</v>
       </c>
     </row>
     <row r="117">
@@ -1654,7 +1654,7 @@
         <v>6</v>
       </c>
       <c r="C117" t="n">
-        <v>444.06849676109</v>
+        <v>444.068496761294</v>
       </c>
     </row>
     <row r="118">
@@ -1665,7 +1665,7 @@
         <v>6</v>
       </c>
       <c r="C118" t="n">
-        <v>444.180256613903</v>
+        <v>444.180256614108</v>
       </c>
     </row>
     <row r="119">
@@ -1676,7 +1676,7 @@
         <v>6</v>
       </c>
       <c r="C119" t="n">
-        <v>443.658724581641</v>
+        <v>443.658724581843</v>
       </c>
     </row>
     <row r="120">
@@ -1687,7 +1687,7 @@
         <v>6</v>
       </c>
       <c r="C120" t="n">
-        <v>444.03452787135</v>
+        <v>444.034527871554</v>
       </c>
     </row>
     <row r="121">
@@ -1698,7 +1698,7 @@
         <v>6</v>
       </c>
       <c r="C121" t="n">
-        <v>443.693044211893</v>
+        <v>443.693044212096</v>
       </c>
     </row>
     <row r="122">
@@ -1709,7 +1709,7 @@
         <v>6</v>
       </c>
       <c r="C122" t="n">
-        <v>444.185168873959</v>
+        <v>444.185168874163</v>
       </c>
     </row>
     <row r="123">
@@ -1720,7 +1720,7 @@
         <v>6</v>
       </c>
       <c r="C123" t="n">
-        <v>444.049201913479</v>
+        <v>444.049201913683</v>
       </c>
     </row>
     <row r="124">
@@ -1731,7 +1731,7 @@
         <v>6</v>
       </c>
       <c r="C124" t="n">
-        <v>444.128800002639</v>
+        <v>444.128800002844</v>
       </c>
     </row>
     <row r="125">
@@ -1742,7 +1742,7 @@
         <v>6</v>
       </c>
       <c r="C125" t="n">
-        <v>444.149260949354</v>
+        <v>444.149260949559</v>
       </c>
     </row>
   </sheetData>

</xml_diff>